<commit_message>
ZSS-697: add 3D support
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/697-chart-engine.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/697-chart-engine.xlsx
@@ -80,13 +80,13 @@
     <t>2. chart should works well. (don't care showing order)</t>
   </si>
   <si>
-    <t>3. known issue: no title, no 3D-surface chart, no stock chart, no ALL 3D model, line and area chart doesn't have stacked or percentage stacked style, no double donut chart.</t>
-  </si>
-  <si>
     <t>4. export without highchart export server, you should see the jfreechart based chart.</t>
   </si>
   <si>
     <t>5. export with highchart export server, you should see the highchart based chart.</t>
+  </si>
+  <si>
+    <t>3. known issue: no title, no double donut chart.</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -271,8 +270,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="234314376"/>
-        <c:axId val="234312416"/>
+        <c:axId val="231470024"/>
+        <c:axId val="232193912"/>
       </c:barChart>
       <c:stockChart>
         <c:ser>
@@ -510,11 +509,11 @@
             <a:effectLst/>
           </c:spPr>
         </c:hiLowLines>
-        <c:axId val="234316336"/>
-        <c:axId val="234311632"/>
+        <c:axId val="232193128"/>
+        <c:axId val="232191952"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="234314376"/>
+        <c:axId val="231470024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +556,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234312416"/>
+        <c:crossAx val="232193912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="234312416"/>
+        <c:axId val="232193912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,12 +615,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234314376"/>
+        <c:crossAx val="231470024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="234311632"/>
+        <c:axId val="232191952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,12 +671,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234316336"/>
+        <c:crossAx val="232193128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="234316336"/>
+        <c:axId val="232193128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +686,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234311632"/>
+        <c:crossAx val="232191952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -704,7 +703,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1018,12 +1016,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="347940592"/>
-        <c:axId val="347940984"/>
+        <c:axId val="5566968"/>
+        <c:axId val="5567360"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="347940592"/>
+        <c:axId val="5566968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1058,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347940984"/>
+        <c:crossAx val="5567360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1068,7 +1066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347940984"/>
+        <c:axId val="5567360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,7 +1117,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347940592"/>
+        <c:crossAx val="5566968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1410,11 +1408,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="348132640"/>
-        <c:axId val="348133032"/>
+        <c:axId val="5568144"/>
+        <c:axId val="5568536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348132640"/>
+        <c:axId val="5568144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1457,7 +1455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348133032"/>
+        <c:crossAx val="5568536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1465,7 +1463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348133032"/>
+        <c:axId val="5568536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1516,7 +1514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348132640"/>
+        <c:crossAx val="5568144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1807,11 +1805,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="348133816"/>
-        <c:axId val="348134208"/>
+        <c:axId val="5569320"/>
+        <c:axId val="5569712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348133816"/>
+        <c:axId val="5569320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348134208"/>
+        <c:crossAx val="5569712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1862,7 +1860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348134208"/>
+        <c:axId val="5569712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1913,7 +1911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348133816"/>
+        <c:crossAx val="5569320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2204,11 +2202,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="348134992"/>
-        <c:axId val="348135384"/>
+        <c:axId val="315293664"/>
+        <c:axId val="315294056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348134992"/>
+        <c:axId val="315293664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348135384"/>
+        <c:crossAx val="315294056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2259,7 +2257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348135384"/>
+        <c:axId val="315294056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2310,7 +2308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348134992"/>
+        <c:crossAx val="315293664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2588,12 +2586,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348389304"/>
-        <c:axId val="348389696"/>
-        <c:axId val="348397496"/>
+        <c:axId val="315294840"/>
+        <c:axId val="315295232"/>
+        <c:axId val="315324896"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="348389304"/>
+        <c:axId val="315294840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,7 +2634,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348389696"/>
+        <c:crossAx val="315295232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2644,7 +2642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348389696"/>
+        <c:axId val="315295232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,12 +2693,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348389304"/>
+        <c:crossAx val="315294840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="348397496"/>
+        <c:axId val="315324896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2742,7 +2740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348389696"/>
+        <c:crossAx val="315295232"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -3023,11 +3021,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348390480"/>
-        <c:axId val="348390872"/>
+        <c:axId val="315296016"/>
+        <c:axId val="315296408"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="348390480"/>
+        <c:axId val="315296016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3070,7 +3068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348390872"/>
+        <c:crossAx val="315296408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3078,7 +3076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348390872"/>
+        <c:axId val="315296408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,7 +3127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348390480"/>
+        <c:crossAx val="315296016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3411,11 +3409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348391656"/>
-        <c:axId val="348392048"/>
+        <c:axId val="319674896"/>
+        <c:axId val="319675288"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="348391656"/>
+        <c:axId val="319674896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3458,7 +3456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348392048"/>
+        <c:crossAx val="319675288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3466,7 +3464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348392048"/>
+        <c:axId val="319675288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,7 +3515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348391656"/>
+        <c:crossAx val="319674896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3799,11 +3797,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348392832"/>
-        <c:axId val="348590016"/>
+        <c:axId val="319676072"/>
+        <c:axId val="319676464"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="348392832"/>
+        <c:axId val="319676072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3846,7 +3844,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348590016"/>
+        <c:crossAx val="319676464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3854,7 +3852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348590016"/>
+        <c:axId val="319676464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3905,7 +3903,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348392832"/>
+        <c:crossAx val="319676072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4241,12 +4239,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="348590800"/>
-        <c:axId val="348591192"/>
-        <c:axId val="348669888"/>
+        <c:axId val="319677248"/>
+        <c:axId val="319677640"/>
+        <c:axId val="319673344"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="348590800"/>
+        <c:axId val="319677248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4289,7 +4287,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348591192"/>
+        <c:crossAx val="319677640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4297,7 +4295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348591192"/>
+        <c:axId val="319677640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4348,12 +4346,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348590800"/>
+        <c:crossAx val="319677248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="348669888"/>
+        <c:axId val="319673344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4395,7 +4393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348591192"/>
+        <c:crossAx val="319677640"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -4902,7 +4900,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5262,11 +5259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="234317904"/>
-        <c:axId val="241146376"/>
+        <c:axId val="205302456"/>
+        <c:axId val="162465904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="234317904"/>
+        <c:axId val="205302456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5322,12 +5319,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241146376"/>
+        <c:crossAx val="162465904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="241146376"/>
+        <c:axId val="162465904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5384,7 +5381,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="234317904"/>
+        <c:crossAx val="205302456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5398,7 +5395,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6393,7 +6389,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6618,11 +6613,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="348593152"/>
-        <c:axId val="348593544"/>
+        <c:axId val="317895000"/>
+        <c:axId val="317895392"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="348593152"/>
+        <c:axId val="317895000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6678,12 +6673,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348593544"/>
+        <c:crossAx val="317895392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="348593544"/>
+        <c:axId val="317895392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6740,7 +6735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348593152"/>
+        <c:crossAx val="317895000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6754,7 +6749,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6836,7 +6830,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7353,12 +7346,12 @@
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
-        <c:axId val="348973400"/>
-        <c:axId val="348973792"/>
-        <c:axId val="349035128"/>
+        <c:axId val="317896176"/>
+        <c:axId val="317896568"/>
+        <c:axId val="322531800"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="348973400"/>
+        <c:axId val="317896176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7401,7 +7394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348973792"/>
+        <c:crossAx val="317896568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7409,7 +7402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348973792"/>
+        <c:axId val="317896568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7460,12 +7453,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348973400"/>
+        <c:crossAx val="317896176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="349035128"/>
+        <c:axId val="322531800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7507,7 +7500,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348973792"/>
+        <c:crossAx val="317896568"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -7566,30 +7559,6 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7862,11 +7831,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="347160600"/>
-        <c:axId val="347160992"/>
+        <c:axId val="319183616"/>
+        <c:axId val="319184008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347160600"/>
+        <c:axId val="319183616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7909,7 +7878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347160992"/>
+        <c:crossAx val="319184008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7917,7 +7886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347160992"/>
+        <c:axId val="319184008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7968,7 +7937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347160600"/>
+        <c:crossAx val="319183616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8255,11 +8224,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="347161776"/>
-        <c:axId val="347162168"/>
+        <c:axId val="319184792"/>
+        <c:axId val="233094280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347161776"/>
+        <c:axId val="319184792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8302,7 +8271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347162168"/>
+        <c:crossAx val="233094280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8310,7 +8279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347162168"/>
+        <c:axId val="233094280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8361,7 +8330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347161776"/>
+        <c:crossAx val="319184792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -8651,11 +8620,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="347160208"/>
-        <c:axId val="347159816"/>
+        <c:axId val="319183224"/>
+        <c:axId val="319182832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347160208"/>
+        <c:axId val="319183224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8698,7 +8667,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347159816"/>
+        <c:crossAx val="319182832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8706,7 +8675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347159816"/>
+        <c:axId val="319182832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8757,7 +8726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347160208"/>
+        <c:crossAx val="319183224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9085,12 +9054,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="347163344"/>
-        <c:axId val="241101320"/>
+        <c:axId val="319182048"/>
+        <c:axId val="319181656"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="347163344"/>
+        <c:axId val="319182048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9127,7 +9096,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241101320"/>
+        <c:crossAx val="319181656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9135,7 +9104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241101320"/>
+        <c:axId val="319181656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9186,7 +9155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347163344"/>
+        <c:crossAx val="319182048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9598,11 +9567,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="196314920"/>
-        <c:axId val="347937456"/>
+        <c:axId val="233095456"/>
+        <c:axId val="233095848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196314920"/>
+        <c:axId val="233095456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9645,7 +9614,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347937456"/>
+        <c:crossAx val="233095848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9653,7 +9622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347937456"/>
+        <c:axId val="233095848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9704,7 +9673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196314920"/>
+        <c:crossAx val="233095456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9991,11 +9960,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="347938240"/>
-        <c:axId val="347938632"/>
+        <c:axId val="233096632"/>
+        <c:axId val="233097024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347938240"/>
+        <c:axId val="233096632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10038,7 +10007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347938632"/>
+        <c:crossAx val="233097024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10046,7 +10015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347938632"/>
+        <c:axId val="233097024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10097,7 +10066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347938240"/>
+        <c:crossAx val="233096632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10384,11 +10353,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="347939416"/>
-        <c:axId val="347939808"/>
+        <c:axId val="233097808"/>
+        <c:axId val="5566184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="347939416"/>
+        <c:axId val="233097808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10431,7 +10400,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347939808"/>
+        <c:crossAx val="5566184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10439,7 +10408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347939808"/>
+        <c:axId val="5566184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10490,7 +10459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="347939416"/>
+        <c:crossAx val="233097808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23700,7 +23669,7 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23730,7 +23699,7 @@
         <v>16</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -23765,7 +23734,7 @@
         <v>17</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -23797,7 +23766,7 @@
         <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>